<commit_message>
Update Sentiment, Key phrase with translation
</commit_message>
<xml_diff>
--- a/inputFiles/Feedback.xlsx
+++ b/inputFiles/Feedback.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mishrarahul/VisualStudioProjects/LanguageAzure/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aviragsrivastava/Downloads/GitHub/languageAzure/inputFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2598E5E-44F3-5F46-8024-586A958B24D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181F321D-5D94-CC49-A4B3-27016C279C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16620" xr2:uid="{6AAD7BF2-D9AB-9446-92CE-B3906FE0A679}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="16180" xr2:uid="{6AAD7BF2-D9AB-9446-92CE-B3906FE0A679}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
-  <si>
-    <t>Text</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t xml:space="preserve"> Sentiment</t>
   </si>
@@ -198,6 +192,15 @@
   </si>
   <si>
     <t xml:space="preserve"> 2023-07-02 10:45:21</t>
+  </si>
+  <si>
+    <t>Positive review</t>
+  </si>
+  <si>
+    <t>Negative review</t>
+  </si>
+  <si>
+    <t>I hate login</t>
   </si>
 </sst>
 </file>
@@ -233,8 +236,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,264 +555,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEE9D459-F563-CD47-B0B9-7F738C6CC504}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:H99"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G3">
-        <v>0.65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G4">
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10">
         <v>0.92</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="E11" t="s">
         <v>52</v>
       </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
         <v>17</v>
       </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11">
+      <c r="H11">
         <v>0.65</v>
       </c>
     </row>

</xml_diff>